<commit_message>
feat(multiplayer): start debug level
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t xml:space="preserve">DÉMARRER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIN_MULTIPLAYER_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTIPLAYER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTI-JOUEUR</t>
   </si>
   <si>
     <t xml:space="preserve">MAIN_CREDITS_BUTTON</t>
@@ -360,10 +369,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,6 +535,17 @@
         <v>40</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(multiplayer): implement lobby to host or join a multiplayer game (#23)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t xml:space="preserve">DÉMARRER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIN_MULTIPLAYER_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTIPLAYER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTI-JOUEUR</t>
   </si>
   <si>
     <t xml:space="preserve">MAIN_CREDITS_BUTTON</t>
@@ -360,10 +369,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,6 +535,17 @@
         <v>40</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
chore: add missing translations in xlsx
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -152,6 +152,69 @@
   </si>
   <si>
     <t xml:space="preserve">RETOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_CHOICE_MENU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose your weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choisis ton arme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_CHOICE_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prendre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_GUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistolet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_SWORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Épée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_ATTRIBUTE_DAMAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dégats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_ATTRIBUTE_RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_ATTRIBUTE_ATTACK_SPEED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitesse d'attaque</t>
   </si>
 </sst>
 </file>
@@ -191,12 +254,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -233,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,6 +319,30 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -255,6 +354,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -369,16 +528,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -393,157 +553,234 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: add missing translations in xlsx (#38)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -152,6 +152,69 @@
   </si>
   <si>
     <t xml:space="preserve">RETOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_CHOICE_MENU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose your weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choisis ton arme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_CHOICE_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prendre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_GUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistolet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_SWORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Épée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_ATTRIBUTE_DAMAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dégats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_ATTRIBUTE_RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAPON_ATTRIBUTE_ATTACK_SPEED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitesse d'attaque</t>
   </si>
 </sst>
 </file>
@@ -191,12 +254,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -233,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,6 +319,30 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -255,6 +354,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -369,16 +528,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -393,157 +553,234 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>